<commit_message>
Solicitud material gráfico versión editada después de borrar el guión
A este archivo se le eliminó la foto No 32.

Se completó la información del esqueleto anterior.
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado07/guion01/SolicitudGraficaCS_07_01_CO.xlsx
+++ b/fuentes/contenidos/grado07/guion01/SolicitudGraficaCS_07_01_CO.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25240" windowHeight="14180" tabRatio="500"/>
+    <workbookView xWindow="20" yWindow="0" windowWidth="25000" windowHeight="14420" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Solicitud gráfica" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="266">
   <si>
     <t>Fecha:</t>
   </si>
@@ -867,9 +867,6 @@
     <t>IMG39</t>
   </si>
   <si>
-    <t>IMG40</t>
-  </si>
-  <si>
     <t>Fotografía</t>
   </si>
   <si>
@@ -904,6 +901,9 @@
   </si>
   <si>
     <t>Foto interior de la iglesia del monasterio de San Miguel de Escala</t>
+  </si>
+  <si>
+    <t>Ilustración</t>
   </si>
 </sst>
 </file>
@@ -1578,7 +1578,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1632,8 +1632,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="107">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1837,6 +1839,7 @@
     <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1921,9 +1924,14 @@
     <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="55">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
@@ -1950,6 +1958,7 @@
     <cellStyle name="Hipervínculo" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="49" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="53" builtinId="8" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
@@ -1976,6 +1985,7 @@
     <cellStyle name="Hipervínculo visitado" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="50" builtinId="9" hidden="1"/>
     <cellStyle name="Hipervínculo visitado" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="54" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="3">
@@ -2670,11 +2680,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1" enableFormatConditionsCalculation="0"/>
-  <dimension ref="A1:P106"/>
+  <dimension ref="A1:P105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E47" sqref="E47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="13" x14ac:dyDescent="0"/>
@@ -2712,14 +2722,14 @@
       <c r="B2" s="65" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="82" t="s">
+      <c r="C2" s="83" t="s">
         <v>23</v>
       </c>
-      <c r="D2" s="83"/>
-      <c r="F2" s="75" t="s">
+      <c r="D2" s="84"/>
+      <c r="F2" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="G2" s="76"/>
+      <c r="G2" s="77"/>
       <c r="H2" s="34"/>
       <c r="I2" s="34"/>
       <c r="J2" s="13"/>
@@ -2729,14 +2739,14 @@
       <c r="B3" s="66" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="84">
+      <c r="C3" s="85">
         <v>7</v>
       </c>
-      <c r="D3" s="85"/>
-      <c r="F3" s="77">
+      <c r="D3" s="86"/>
+      <c r="F3" s="78">
         <v>42071</v>
       </c>
-      <c r="G3" s="78"/>
+      <c r="G3" s="79"/>
       <c r="H3" s="34"/>
       <c r="I3" s="34"/>
       <c r="J3" s="13"/>
@@ -2746,10 +2756,10 @@
       <c r="B4" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="85" t="s">
         <v>145</v>
       </c>
-      <c r="D4" s="85"/>
+      <c r="D4" s="86"/>
       <c r="E4" s="3"/>
       <c r="F4" s="68" t="s">
         <v>55</v>
@@ -2767,10 +2777,10 @@
       <c r="B5" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="86" t="s">
+      <c r="C5" s="87" t="s">
         <v>150</v>
       </c>
-      <c r="D5" s="87"/>
+      <c r="D5" s="88"/>
       <c r="E5" s="3"/>
       <c r="F5" s="32" t="str">
         <f>IF(G4="Recurso","Motor del recurso","")</f>
@@ -2819,12 +2829,12 @@
       <c r="C8" s="7"/>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
-      <c r="F8" s="79" t="s">
+      <c r="F8" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="G8" s="80"/>
-      <c r="H8" s="80"/>
-      <c r="I8" s="81"/>
+      <c r="G8" s="81"/>
+      <c r="H8" s="81"/>
+      <c r="I8" s="82"/>
       <c r="J8" s="15"/>
       <c r="K8" s="9"/>
       <c r="L8" s="2"/>
@@ -2880,10 +2890,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D10" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E10" s="11" t="s">
         <v>254</v>
-      </c>
-      <c r="E10" s="11" t="s">
-        <v>255</v>
       </c>
       <c r="F10" s="11" t="str">
         <f t="shared" ref="F10" si="1">IF(OR(B10&lt;&gt;"",J10&lt;&gt;""),CONCATENATE($C$7,"_",$A10,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I10="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
@@ -2905,7 +2915,7 @@
         <v>149</v>
       </c>
       <c r="K10" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="11" spans="1:16" s="9" customFormat="1" ht="44">
@@ -2916,17 +2926,17 @@
         <v>151</v>
       </c>
       <c r="C11" s="17" t="str">
-        <f t="shared" ref="C11:C74" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <f t="shared" ref="C11:C73" si="3">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="E11" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F11" s="11" t="str">
-        <f t="shared" ref="F11:F72" si="4">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" ref="F11:F71" si="4">IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I11="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v>CS_07_01_CO_IMG02_small</v>
       </c>
       <c r="G11" s="11" t="str">
@@ -2934,7 +2944,7 @@
         <v>526 x 370 px</v>
       </c>
       <c r="H11" s="11" t="str">
-        <f t="shared" ref="H11:H72" si="5">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" ref="H11:H71" si="5">IF(AND(I11&lt;&gt;"",I11&lt;&gt;0),IF(OR(B11&lt;&gt;"",J11&lt;&gt;""),CONCATENATE($C$7,"_",$A11,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v>CS_07_01_CO_IMG02_zoom</v>
       </c>
       <c r="I11" s="11" t="str">
@@ -2945,7 +2955,7 @@
         <v>152</v>
       </c>
       <c r="K11" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" spans="1:16" s="9" customFormat="1" ht="44">
@@ -2960,10 +2970,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F12" s="11" t="str">
         <f t="shared" si="4"/>
@@ -2985,7 +2995,7 @@
         <v>154</v>
       </c>
       <c r="K12" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:16" s="9" customFormat="1" ht="56" thickBot="1">
@@ -3000,10 +3010,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F13" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3025,7 +3035,7 @@
         <v>155</v>
       </c>
       <c r="K13" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="14" spans="1:16" s="9" customFormat="1" ht="34" thickBot="1">
@@ -3040,10 +3050,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D14" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="E14" s="11" t="s">
         <v>254</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>255</v>
       </c>
       <c r="F14" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3065,7 +3075,7 @@
         <v>158</v>
       </c>
       <c r="K14" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="15" spans="1:16" s="9" customFormat="1" ht="34" thickBot="1">
@@ -3080,10 +3090,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D15" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E15" s="11" t="s">
         <v>254</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>255</v>
       </c>
       <c r="F15" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3105,7 +3115,7 @@
         <v>159</v>
       </c>
       <c r="K15" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:16" s="9" customFormat="1" ht="34" thickBot="1">
@@ -3120,10 +3130,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F16" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3145,7 +3155,7 @@
         <v>160</v>
       </c>
       <c r="K16" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="9" customFormat="1" ht="33">
@@ -3160,10 +3170,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F17" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3185,7 +3195,7 @@
         <v>163</v>
       </c>
       <c r="K17" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="9" customFormat="1" ht="44">
@@ -3200,10 +3210,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D18" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E18" s="11" t="s">
         <v>254</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>255</v>
       </c>
       <c r="F18" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3225,7 +3235,7 @@
         <v>165</v>
       </c>
       <c r="K18" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="9" customFormat="1" ht="22">
@@ -3240,10 +3250,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F19" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3265,7 +3275,7 @@
         <v>167</v>
       </c>
       <c r="K19" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="9" customFormat="1" ht="33">
@@ -3280,10 +3290,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F20" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3305,7 +3315,7 @@
         <v>169</v>
       </c>
       <c r="K20" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="21" spans="1:11" s="9" customFormat="1" ht="45" thickBot="1">
@@ -3320,10 +3330,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F21" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3345,7 +3355,7 @@
         <v>170</v>
       </c>
       <c r="K21" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="22" spans="1:11" s="9" customFormat="1" ht="45" thickBot="1">
@@ -3360,10 +3370,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F22" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3385,7 +3395,7 @@
         <v>173</v>
       </c>
       <c r="K22" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="23" spans="1:11" s="9" customFormat="1" ht="44">
@@ -3400,10 +3410,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F23" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3425,7 +3435,7 @@
         <v>175</v>
       </c>
       <c r="K23" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="9" customFormat="1" ht="34" thickBot="1">
@@ -3440,10 +3450,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F24" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3465,7 +3475,7 @@
         <v>177</v>
       </c>
       <c r="K24" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="9" customFormat="1" ht="34" thickBot="1">
@@ -3480,10 +3490,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F25" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3505,7 +3515,7 @@
         <v>179</v>
       </c>
       <c r="K25" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="9" customFormat="1" ht="33">
@@ -3520,10 +3530,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F26" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3545,7 +3555,7 @@
         <v>180</v>
       </c>
       <c r="K26" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="9" customFormat="1" ht="45" thickBot="1">
@@ -3560,10 +3570,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F27" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3585,7 +3595,7 @@
         <v>182</v>
       </c>
       <c r="K27" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="28" spans="1:11" s="9" customFormat="1" ht="56" thickBot="1">
@@ -3600,10 +3610,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F28" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3625,7 +3635,7 @@
         <v>184</v>
       </c>
       <c r="K28" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="29" spans="1:11" s="9" customFormat="1" ht="44">
@@ -3640,10 +3650,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D29" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E29" s="11" t="s">
         <v>254</v>
-      </c>
-      <c r="E29" s="11" t="s">
-        <v>255</v>
       </c>
       <c r="F29" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3665,7 +3675,7 @@
         <v>186</v>
       </c>
       <c r="K29" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="30" spans="1:11" s="9" customFormat="1" ht="55">
@@ -3680,10 +3690,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F30" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3705,7 +3715,7 @@
         <v>188</v>
       </c>
       <c r="K30" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="31" spans="1:11" s="9" customFormat="1" ht="34" thickBot="1">
@@ -3720,10 +3730,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F31" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3745,7 +3755,7 @@
         <v>190</v>
       </c>
       <c r="K31" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="32" spans="1:11" s="9" customFormat="1" ht="23" thickBot="1">
@@ -3760,10 +3770,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F32" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3785,7 +3795,7 @@
         <v>192</v>
       </c>
       <c r="K32" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="9" customFormat="1" ht="33">
@@ -3800,10 +3810,10 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F33" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3825,25 +3835,25 @@
         <v>194</v>
       </c>
       <c r="K33" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="9" customFormat="1" ht="15">
       <c r="A34" s="62" t="s">
         <v>238</v>
       </c>
-      <c r="B34" s="106" t="s">
-        <v>258</v>
+      <c r="B34" s="75" t="s">
+        <v>257</v>
       </c>
       <c r="C34" s="17" t="str">
         <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
       <c r="E34" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F34" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3861,29 +3871,29 @@
         <f>IF(OR(B34&lt;&gt;"",J34&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J34" s="106" t="s">
+      <c r="J34" s="75" t="s">
         <v>195</v>
       </c>
       <c r="K34" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="9" customFormat="1" ht="15">
       <c r="A35" s="62" t="s">
         <v>239</v>
       </c>
-      <c r="B35" s="106" t="s">
-        <v>259</v>
+      <c r="B35" s="75" t="s">
+        <v>258</v>
       </c>
       <c r="C35" s="17" t="str">
         <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E35" s="11" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="F35" s="11" t="str">
         <f t="shared" si="4"/>
@@ -3901,28 +3911,30 @@
         <f>IF(OR(B35&lt;&gt;"",J35&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J35" s="106" t="s">
-        <v>260</v>
+      <c r="J35" s="75" t="s">
+        <v>259</v>
       </c>
       <c r="K35" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="9" customFormat="1" ht="15">
       <c r="A36" s="62" t="s">
         <v>240</v>
       </c>
-      <c r="B36" s="106" t="s">
-        <v>261</v>
+      <c r="B36" s="75" t="s">
+        <v>260</v>
       </c>
       <c r="C36" s="17" t="str">
         <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="E36" s="11"/>
+        <v>265</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>255</v>
+      </c>
       <c r="F36" s="11" t="str">
         <f t="shared" si="4"/>
         <v>CS_07_01_CO_IMG27_small</v>
@@ -3939,28 +3951,30 @@
         <f>IF(OR(B36&lt;&gt;"",J36&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J36" s="106" t="s">
+      <c r="J36" s="75" t="s">
         <v>196</v>
       </c>
       <c r="K36" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="9" customFormat="1" ht="15">
       <c r="A37" s="62" t="s">
         <v>241</v>
       </c>
-      <c r="B37" s="106" t="s">
-        <v>262</v>
+      <c r="B37" s="75" t="s">
+        <v>261</v>
       </c>
       <c r="C37" s="17" t="str">
         <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D37" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E37" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E37" s="11"/>
       <c r="F37" s="11" t="str">
         <f t="shared" si="4"/>
         <v>CS_07_01_CO_IMG28_small</v>
@@ -3977,28 +3991,30 @@
         <f>IF(OR(B37&lt;&gt;"",J37&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J37" s="106" t="s">
+      <c r="J37" s="75" t="s">
         <v>197</v>
       </c>
       <c r="K37" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="9" customFormat="1" ht="15">
       <c r="A38" s="62" t="s">
         <v>242</v>
       </c>
-      <c r="B38" s="106" t="s">
-        <v>263</v>
+      <c r="B38" s="75" t="s">
+        <v>262</v>
       </c>
       <c r="C38" s="17" t="str">
         <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D38" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E38" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E38" s="11"/>
       <c r="F38" s="11" t="str">
         <f t="shared" si="4"/>
         <v>CS_07_01_CO_IMG29_small</v>
@@ -4015,28 +4031,30 @@
         <f>IF(OR(B38&lt;&gt;"",J38&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J38" s="106" t="s">
+      <c r="J38" s="75" t="s">
         <v>198</v>
       </c>
       <c r="K38" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="39" spans="1:11" s="9" customFormat="1" ht="15">
       <c r="A39" s="62" t="s">
         <v>243</v>
       </c>
-      <c r="B39" s="106" t="s">
-        <v>264</v>
+      <c r="B39" s="75" t="s">
+        <v>263</v>
       </c>
       <c r="C39" s="17" t="str">
         <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D39" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E39" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E39" s="11"/>
       <c r="F39" s="11" t="str">
         <f t="shared" si="4"/>
         <v>CS_07_01_CO_IMG30_small</v>
@@ -4053,11 +4071,11 @@
         <f>IF(OR(B39&lt;&gt;"",J39&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J39" s="106" t="s">
-        <v>265</v>
+      <c r="J39" s="75" t="s">
+        <v>264</v>
       </c>
       <c r="K39" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="9" customFormat="1" ht="46" thickBot="1">
@@ -4072,9 +4090,11 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="E40" s="11"/>
+        <v>265</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>255</v>
+      </c>
       <c r="F40" s="11" t="str">
         <f t="shared" si="4"/>
         <v>CS_07_01_CO_IMG31_small</v>
@@ -4091,28 +4111,30 @@
         <f>IF(OR(B40&lt;&gt;"",J40&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J40" s="106" t="s">
+      <c r="J40" s="75" t="s">
         <v>200</v>
       </c>
       <c r="K40" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="41" spans="1:11" s="9" customFormat="1" ht="45" thickBot="1">
       <c r="A41" s="62" t="s">
         <v>245</v>
       </c>
-      <c r="B41" s="57" t="s">
-        <v>199</v>
+      <c r="B41" s="107" t="s">
+        <v>201</v>
       </c>
       <c r="C41" s="17" t="str">
         <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="E41" s="11"/>
+        <v>265</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>255</v>
+      </c>
       <c r="F41" s="11" t="str">
         <f t="shared" si="4"/>
         <v>CS_07_01_CO_IMG32_small</v>
@@ -4129,11 +4151,11 @@
         <f>IF(OR(B41&lt;&gt;"",J41&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J41" s="59" t="s">
-        <v>200</v>
-      </c>
-      <c r="K41" s="59" t="s">
-        <v>257</v>
+      <c r="J41" s="108" t="s">
+        <v>202</v>
+      </c>
+      <c r="K41" s="107" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="42" spans="1:11" s="9" customFormat="1" ht="45" thickBot="1">
@@ -4148,7 +4170,7 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="E42" s="11"/>
       <c r="F42" s="11" t="str">
@@ -4168,27 +4190,29 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J42" s="57" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="K42" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="9" customFormat="1" ht="45" thickBot="1">
       <c r="A43" s="62" t="s">
         <v>247</v>
       </c>
-      <c r="B43" s="59" t="s">
-        <v>201</v>
+      <c r="B43" s="57" t="s">
+        <v>204</v>
       </c>
       <c r="C43" s="17" t="str">
         <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D43" s="11" t="s">
+        <v>253</v>
+      </c>
+      <c r="E43" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E43" s="11"/>
       <c r="F43" s="11" t="str">
         <f t="shared" si="4"/>
         <v>CS_07_01_CO_IMG34_small</v>
@@ -4205,18 +4229,18 @@
         <f>IF(OR(B43&lt;&gt;"",J43&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J43" s="57" t="s">
-        <v>203</v>
+      <c r="J43" s="58" t="s">
+        <v>205</v>
       </c>
       <c r="K43" s="59" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="44" spans="1:11" s="9" customFormat="1" ht="45" thickBot="1">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" s="9" customFormat="1" ht="44">
       <c r="A44" s="62" t="s">
         <v>248</v>
       </c>
-      <c r="B44" s="57" t="s">
+      <c r="B44" s="59" t="s">
         <v>204</v>
       </c>
       <c r="C44" s="17" t="str">
@@ -4224,9 +4248,11 @@
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="E44" s="11"/>
+        <v>253</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>255</v>
+      </c>
       <c r="F44" s="11" t="str">
         <f t="shared" si="4"/>
         <v>CS_07_01_CO_IMG35_small</v>
@@ -4244,10 +4270,10 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J44" s="58" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="K44" s="59" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="45" spans="1:11" s="9" customFormat="1" ht="44">
@@ -4255,16 +4281,18 @@
         <v>249</v>
       </c>
       <c r="B45" s="59" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="C45" s="17" t="str">
         <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D45" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="E45" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E45" s="11"/>
       <c r="F45" s="11" t="str">
         <f t="shared" si="4"/>
         <v>CS_07_01_CO_IMG36_small</v>
@@ -4282,27 +4310,29 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J45" s="58" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="K45" s="59" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="46" spans="1:11" s="9" customFormat="1" ht="44">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" s="9" customFormat="1" ht="45" thickBot="1">
       <c r="A46" s="62" t="s">
         <v>250</v>
       </c>
       <c r="B46" s="59" t="s">
-        <v>207</v>
+        <v>209</v>
       </c>
       <c r="C46" s="17" t="str">
         <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D46" s="11" t="s">
+        <v>265</v>
+      </c>
+      <c r="E46" s="11" t="s">
         <v>254</v>
       </c>
-      <c r="E46" s="11"/>
       <c r="F46" s="11" t="str">
         <f t="shared" si="4"/>
         <v>CS_07_01_CO_IMG37_small</v>
@@ -4320,27 +4350,29 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J46" s="58" t="s">
-        <v>208</v>
+        <v>210</v>
       </c>
       <c r="K46" s="59" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" s="9" customFormat="1" ht="45" thickBot="1">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="9" customFormat="1" ht="34" thickBot="1">
       <c r="A47" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="B47" s="59" t="s">
-        <v>209</v>
+      <c r="B47" s="57" t="s">
+        <v>211</v>
       </c>
       <c r="C47" s="17" t="str">
         <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="E47" s="11"/>
+        <v>253</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>255</v>
+      </c>
       <c r="F47" s="11" t="str">
         <f t="shared" si="4"/>
         <v>CS_07_01_CO_IMG38_small</v>
@@ -4357,28 +4389,30 @@
         <f>IF(OR(B47&lt;&gt;"",J47&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
         <v>800 x 600 px</v>
       </c>
-      <c r="J47" s="58" t="s">
-        <v>210</v>
+      <c r="J47" s="59" t="s">
+        <v>212</v>
       </c>
       <c r="K47" s="59" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="48" spans="1:11" s="9" customFormat="1" ht="34" thickBot="1">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" s="9" customFormat="1" ht="55">
       <c r="A48" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="B48" s="57" t="s">
-        <v>211</v>
+      <c r="B48" s="59" t="s">
+        <v>213</v>
       </c>
       <c r="C48" s="17" t="str">
         <f t="shared" si="3"/>
         <v>Cuaderno de Estudio</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="E48" s="11"/>
+        <v>265</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>255</v>
+      </c>
       <c r="F48" s="11" t="str">
         <f t="shared" si="4"/>
         <v>CS_07_01_CO_IMG39_small</v>
@@ -4396,49 +4430,39 @@
         <v>800 x 600 px</v>
       </c>
       <c r="J48" s="59" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="K48" s="59" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="49" spans="1:11" s="9" customFormat="1" ht="55">
-      <c r="A49" s="62" t="s">
-        <v>253</v>
-      </c>
-      <c r="B49" s="59" t="s">
-        <v>213</v>
-      </c>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" s="9" customFormat="1">
+      <c r="A49" s="17"/>
+      <c r="B49" s="17"/>
       <c r="C49" s="17" t="str">
         <f t="shared" si="3"/>
-        <v>Cuaderno de Estudio</v>
-      </c>
-      <c r="D49" s="11" t="s">
-        <v>254</v>
-      </c>
+        <v/>
+      </c>
+      <c r="D49" s="11"/>
       <c r="E49" s="11"/>
       <c r="F49" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>CS_07_01_CO_IMG40_small</v>
+        <v/>
       </c>
       <c r="G49" s="11" t="str">
         <f>IF(F49&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v>526 x 370 px</v>
+        <v/>
       </c>
       <c r="H49" s="11" t="str">
         <f t="shared" si="5"/>
-        <v>CS_07_01_CO_IMG40_zoom</v>
+        <v/>
       </c>
       <c r="I49" s="11" t="str">
         <f>IF(OR(B49&lt;&gt;"",J49&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v>800 x 600 px</v>
-      </c>
-      <c r="J49" s="59" t="s">
-        <v>214</v>
-      </c>
-      <c r="K49" s="59" t="s">
-        <v>257</v>
-      </c>
+        <v/>
+      </c>
+      <c r="J49" s="11"/>
+      <c r="K49" s="12"/>
     </row>
     <row r="50" spans="1:11" s="9" customFormat="1">
       <c r="A50" s="17"/>
@@ -4694,7 +4718,7 @@
     </row>
     <row r="59" spans="1:11" s="9" customFormat="1">
       <c r="A59" s="17"/>
-      <c r="B59" s="17"/>
+      <c r="B59" s="10"/>
       <c r="C59" s="17" t="str">
         <f t="shared" si="3"/>
         <v/>
@@ -5066,7 +5090,7 @@
       <c r="D72" s="11"/>
       <c r="E72" s="11"/>
       <c r="F72" s="11" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="F72:F105" si="6">IF(OR(B72&lt;&gt;"",J72&lt;&gt;""),CONCATENATE($C$7,"_",$A72,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I72="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
         <v/>
       </c>
       <c r="G72" s="11" t="str">
@@ -5074,7 +5098,7 @@
         <v/>
       </c>
       <c r="H72" s="11" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="H72:H105" si="7">IF(AND(I72&lt;&gt;"",I72&lt;&gt;0),IF(OR(B72&lt;&gt;"",J72&lt;&gt;""),CONCATENATE($C$7,"_",$A72,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
         <v/>
       </c>
       <c r="I72" s="11" t="str">
@@ -5094,7 +5118,7 @@
       <c r="D73" s="11"/>
       <c r="E73" s="11"/>
       <c r="F73" s="11" t="str">
-        <f t="shared" ref="F73:F106" si="6">IF(OR(B73&lt;&gt;"",J73&lt;&gt;""),CONCATENATE($C$7,"_",$A73,IF($G$4="Cuaderno de Estudio","_small",CONCATENATE(IF(I73="","","n"),IF(LEFT($G$5,1)="F",".jpg",".png")))),"")</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="G73" s="11" t="str">
@@ -5102,7 +5126,7 @@
         <v/>
       </c>
       <c r="H73" s="11" t="str">
-        <f t="shared" ref="H73:H106" si="7">IF(AND(I73&lt;&gt;"",I73&lt;&gt;0),IF(OR(B73&lt;&gt;"",J73&lt;&gt;""),CONCATENATE($C$7,"_",$A73,IF($G$4="Cuaderno de Estudio","_zoom",CONCATENATE("a",IF(LEFT($G$5,1)="F",".jpg",".png")))),""),"")</f>
+        <f t="shared" si="7"/>
         <v/>
       </c>
       <c r="I73" s="11" t="str">
@@ -5116,7 +5140,7 @@
       <c r="A74" s="17"/>
       <c r="B74" s="10"/>
       <c r="C74" s="17" t="str">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="C74:C105" si="8">IF(OR(B74&lt;&gt;"",J74&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
         <v/>
       </c>
       <c r="D74" s="11"/>
@@ -5144,7 +5168,7 @@
       <c r="A75" s="17"/>
       <c r="B75" s="10"/>
       <c r="C75" s="17" t="str">
-        <f t="shared" ref="C75:C106" si="8">IF(OR(B75&lt;&gt;"",J75&lt;&gt;""),IF($G$4="Recurso",CONCATENATE($G$4," ",$G$5),$G$4),"")</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="D75" s="11"/>
@@ -6007,34 +6031,6 @@
       </c>
       <c r="J105" s="11"/>
       <c r="K105" s="12"/>
-    </row>
-    <row r="106" spans="1:11" s="9" customFormat="1">
-      <c r="A106" s="17"/>
-      <c r="B106" s="10"/>
-      <c r="C106" s="17" t="str">
-        <f t="shared" si="8"/>
-        <v/>
-      </c>
-      <c r="D106" s="11"/>
-      <c r="E106" s="11"/>
-      <c r="F106" s="11" t="str">
-        <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="G106" s="11" t="str">
-        <f>IF(F106&lt;&gt;"",IF($G$4="Recurso",IF(LEFT($G$5,1)="M",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,5,FALSE),IF($G$5="F1",'Definición técnica de imagenes'!$E$15,'Definición técnica de imagenes'!$F$13)),'Definición técnica de imagenes'!$E$16),"")</f>
-        <v/>
-      </c>
-      <c r="H106" s="11" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-      <c r="I106" s="11" t="str">
-        <f>IF(OR(B106&lt;&gt;"",J106&lt;&gt;""),IF($G$4="Recurso",IF(LEFT($G$5,1)="M",IF(VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)=0,"",VLOOKUP($G$5,'Definición técnica de imagenes'!$A$3:$G$17,6,FALSE)),IF($G$5="F1","","")),'Definición técnica de imagenes'!$F$16),"")</f>
-        <v/>
-      </c>
-      <c r="J106" s="11"/>
-      <c r="K106" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -6077,14 +6073,15 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
       <formula1>"3,4,5,6,7,8,9,10,11"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E106">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E10:E105">
       <formula1>"Vertical,Horizontal"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D106">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D10:D105">
       <formula1>"Ilustración,Fotografía"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -6114,25 +6111,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="16" thickBot="1">
-      <c r="A1" s="90" t="s">
+      <c r="A1" s="91" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="91"/>
-      <c r="C1" s="91"/>
-      <c r="D1" s="91"/>
-      <c r="E1" s="91"/>
-      <c r="F1" s="92"/>
+      <c r="B1" s="92"/>
+      <c r="C1" s="92"/>
+      <c r="D1" s="92"/>
+      <c r="E1" s="92"/>
+      <c r="F1" s="93"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="25" t="s">
         <v>42</v>
       </c>
       <c r="B2" s="26"/>
-      <c r="C2" s="93" t="s">
+      <c r="C2" s="94" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="94"/>
-      <c r="E2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="96"/>
       <c r="F2" s="27"/>
     </row>
     <row r="3" spans="1:11" ht="60">
@@ -6140,11 +6137,11 @@
         <v>43</v>
       </c>
       <c r="B3" s="26"/>
-      <c r="C3" s="99" t="s">
+      <c r="C3" s="100" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="100"/>
-      <c r="E3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="102"/>
       <c r="F3" s="27"/>
       <c r="H3" s="18" t="s">
         <v>18</v>
@@ -6195,11 +6192,11 @@
       <c r="C5" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="102" t="str">
+      <c r="D5" s="103" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_CO")</f>
         <v>LE_07_04_CO</v>
       </c>
-      <c r="E5" s="103"/>
+      <c r="E5" s="104"/>
       <c r="F5" s="27"/>
       <c r="H5" s="18" t="s">
         <v>22</v>
@@ -6244,12 +6241,12 @@
       <c r="C7" s="55" t="s">
         <v>127</v>
       </c>
-      <c r="D7" s="88" t="str">
+      <c r="D7" s="89" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D5,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_CO.xls</v>
       </c>
-      <c r="E7" s="88"/>
-      <c r="F7" s="89"/>
+      <c r="E7" s="89"/>
+      <c r="F7" s="90"/>
       <c r="H7" s="18" t="s">
         <v>24</v>
       </c>
@@ -6343,14 +6340,14 @@
       </c>
     </row>
     <row r="13" spans="1:11">
-      <c r="A13" s="90" t="s">
+      <c r="A13" s="91" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="91"/>
-      <c r="C13" s="91"/>
-      <c r="D13" s="91"/>
-      <c r="E13" s="91"/>
-      <c r="F13" s="92"/>
+      <c r="B13" s="92"/>
+      <c r="C13" s="92"/>
+      <c r="D13" s="92"/>
+      <c r="E13" s="92"/>
+      <c r="F13" s="93"/>
       <c r="I13" s="18" t="s">
         <v>33</v>
       </c>
@@ -6383,12 +6380,12 @@
         <v>46</v>
       </c>
       <c r="B15" s="26"/>
-      <c r="C15" s="93" t="s">
+      <c r="C15" s="94" t="s">
         <v>49</v>
       </c>
-      <c r="D15" s="94"/>
-      <c r="E15" s="94"/>
-      <c r="F15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="95"/>
+      <c r="F15" s="96"/>
       <c r="J15" s="18">
         <v>12</v>
       </c>
@@ -6428,12 +6425,12 @@
       <c r="C17" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="D17" s="96" t="str">
+      <c r="D17" s="97" t="str">
         <f>CONCATENATE(H21,"_",I21,"_",J21,"_",K45)</f>
         <v>LE_07_04_REC10</v>
       </c>
-      <c r="E17" s="97"/>
-      <c r="F17" s="98"/>
+      <c r="E17" s="98"/>
+      <c r="F17" s="99"/>
       <c r="J17" s="18">
         <v>14</v>
       </c>
@@ -6449,12 +6446,12 @@
       <c r="C18" s="55" t="s">
         <v>128</v>
       </c>
-      <c r="D18" s="88" t="str">
+      <c r="D18" s="89" t="str">
         <f>CONCATENATE("SolicitudGrafica_",D17,".xls")</f>
         <v>SolicitudGrafica_LE_07_04_REC10.xls</v>
       </c>
-      <c r="E18" s="88"/>
-      <c r="F18" s="89"/>
+      <c r="E18" s="89"/>
+      <c r="F18" s="90"/>
       <c r="J18" s="18">
         <v>15</v>
       </c>
@@ -6858,41 +6855,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="104" t="s">
+      <c r="A1" s="105" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="104" t="s">
+      <c r="B1" s="105" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="104" t="s">
+      <c r="C1" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="D1" s="104" t="s">
+      <c r="D1" s="105" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="104" t="s">
+      <c r="E1" s="105" t="s">
         <v>65</v>
       </c>
-      <c r="F1" s="104" t="s">
+      <c r="F1" s="105" t="s">
         <v>66</v>
       </c>
-      <c r="G1" s="104" t="s">
+      <c r="G1" s="105" t="s">
         <v>67</v>
       </c>
-      <c r="H1" s="105" t="s">
+      <c r="H1" s="106" t="s">
         <v>68</v>
       </c>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
+      <c r="I1" s="106"/>
+      <c r="J1" s="106"/>
     </row>
     <row r="2" spans="1:11">
-      <c r="A2" s="104"/>
-      <c r="B2" s="104"/>
-      <c r="C2" s="104"/>
-      <c r="D2" s="104"/>
-      <c r="E2" s="104"/>
-      <c r="F2" s="104"/>
-      <c r="G2" s="104"/>
+      <c r="A2" s="105"/>
+      <c r="B2" s="105"/>
+      <c r="C2" s="105"/>
+      <c r="D2" s="105"/>
+      <c r="E2" s="105"/>
+      <c r="F2" s="105"/>
+      <c r="G2" s="105"/>
       <c r="H2" s="35" t="s">
         <v>65</v>
       </c>

</xml_diff>